<commit_message>
updated a column header
</commit_message>
<xml_diff>
--- a/ROV_data/2018 SJI area swept estimates_17May2021.xlsx
+++ b/ROV_data/2018 SJI area swept estimates_17May2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pacunrep\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\ZNY333GT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markusmin/Documents/ESA_RF_2021/ROV_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB35A8BD-8234-4634-A6AA-B58A69A07D84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E78B2D1-0906-C742-A30C-56C2531C8F29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4635" yWindow="1035" windowWidth="21600" windowHeight="13815" xr2:uid="{EF322C34-5DA4-485F-990B-86ECAEE6C8E3}"/>
+    <workbookView xWindow="-23480" yWindow="3240" windowWidth="22360" windowHeight="16220" xr2:uid="{EF322C34-5DA4-485F-990B-86ECAEE6C8E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="67">
   <si>
     <t>2018 SJI area swept estimates</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>only 94 points - does not meet outlier editing threshold - not sure what to do with this one yet (5/17/21) - will probably need to use vessel track to create proxy</t>
+  </si>
+  <si>
+    <t>Tran_ID</t>
   </si>
 </sst>
 </file>
@@ -620,22 +623,24 @@
   <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>62</v>
       </c>
@@ -646,7 +651,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -667,7 +672,7 @@
         <v>2.0825877450433525</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -688,7 +693,7 @@
         <v>2.3666465748150891</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -709,7 +714,7 @@
         <v>2.3922911561943918</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -730,7 +735,7 @@
         <v>2.6917229042886923</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -751,7 +756,7 @@
         <v>2.06320401230961</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -772,7 +777,7 @@
         <v>2.3046924023793012</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -793,7 +798,7 @@
         <v>2.3949582307056878</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -814,7 +819,7 @@
         <v>1.836611202242733</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>63</v>
       </c>
@@ -827,7 +832,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -848,7 +853,7 @@
         <v>3.1699496438131347</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -869,7 +874,7 @@
         <v>2.5933668961468892</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -890,7 +895,7 @@
         <v>2.039380587731102</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -911,7 +916,7 @@
         <v>1.468305894443819</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -932,7 +937,7 @@
         <v>1.7733116665588329</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -953,7 +958,7 @@
         <v>2.2247941805919549</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
@@ -974,7 +979,7 @@
         <v>1.6124147540707876</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -995,7 +1000,7 @@
         <v>1.8737700329027442</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
@@ -1016,7 +1021,7 @@
         <v>2.2571694525990234</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
@@ -1037,7 +1042,7 @@
         <v>1.8706490939757723</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>19</v>
       </c>
@@ -1052,7 +1057,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
@@ -1073,7 +1078,7 @@
         <v>2.4606734407663198</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -1094,7 +1099,7 @@
         <v>2.2873154431248341</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -1115,7 +1120,7 @@
         <v>2.1637238144148934</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
@@ -1136,7 +1141,7 @@
         <v>2.2202120949438924</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
@@ -1157,7 +1162,7 @@
         <v>1.4516377009248544</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -1178,7 +1183,7 @@
         <v>2.0151783043599454</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
@@ -1199,7 +1204,7 @@
         <v>2.9731377225792084</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
@@ -1220,7 +1225,7 @@
         <v>1.5087702193585693</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
@@ -1241,7 +1246,7 @@
         <v>2.9426843258336195</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
@@ -1262,7 +1267,7 @@
         <v>1.8968507261211893</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>30</v>
       </c>
@@ -1283,7 +1288,7 @@
         <v>1.675547768849535</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>31</v>
       </c>
@@ -1304,7 +1309,7 @@
         <v>2.3164518003925889</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>32</v>
       </c>
@@ -1325,7 +1330,7 @@
         <v>1.8662581211327274</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>33</v>
       </c>
@@ -1346,7 +1351,7 @@
         <v>2.5134482680103911</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
@@ -1367,7 +1372,7 @@
         <v>1.8122871554893862</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>35</v>
       </c>
@@ -1388,7 +1393,7 @@
         <v>3.1172616735537884</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>36</v>
       </c>
@@ -1409,7 +1414,7 @@
         <v>2.238474183280645</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>37</v>
       </c>
@@ -1430,7 +1435,7 @@
         <v>1.8086791191376446</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>38</v>
       </c>
@@ -1451,7 +1456,7 @@
         <v>1.5303498273341369</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>39</v>
       </c>
@@ -1472,7 +1477,7 @@
         <v>3.3977132623474096</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>40</v>
       </c>
@@ -1493,7 +1498,7 @@
         <v>2.1003450663164931</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>41</v>
       </c>
@@ -1514,7 +1519,7 @@
         <v>2.1526607462351284</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>42</v>
       </c>
@@ -1535,7 +1540,7 @@
         <v>1.5351146305578993</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>43</v>
       </c>
@@ -1556,7 +1561,7 @@
         <v>2.2712940412867244</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>44</v>
       </c>
@@ -1577,7 +1582,7 @@
         <v>2.2705327729413387</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>45</v>
       </c>
@@ -1598,7 +1603,7 @@
         <v>2.6118675651833541</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>46</v>
       </c>
@@ -1619,7 +1624,7 @@
         <v>2.2637226751945749</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>47</v>
       </c>
@@ -1640,7 +1645,7 @@
         <v>2.1909695712585679</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>48</v>
       </c>
@@ -1661,7 +1666,7 @@
         <v>1.7006338983116265</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>49</v>
       </c>
@@ -1682,7 +1687,7 @@
         <v>1.7773215094844381</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>50</v>
       </c>
@@ -1703,7 +1708,7 @@
         <v>2.8972152085408438</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>51</v>
       </c>
@@ -1724,7 +1729,7 @@
         <v>1.790837720764662</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>52</v>
       </c>
@@ -1745,7 +1750,7 @@
         <v>1.2690653692050464</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>53</v>
       </c>
@@ -1766,7 +1771,7 @@
         <v>2.2365632971531797</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>54</v>
       </c>
@@ -1787,7 +1792,7 @@
         <v>2.2737232474447651</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>55</v>
       </c>
@@ -1808,7 +1813,7 @@
         <v>1.9713191688579217</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>56</v>
       </c>
@@ -1829,7 +1834,7 @@
         <v>1.2418042529845257</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>57</v>
       </c>
@@ -1850,7 +1855,7 @@
         <v>1.6681313457660094</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>58</v>
       </c>
@@ -1871,7 +1876,7 @@
         <v>1.8272441472535419</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>59</v>
       </c>
@@ -1892,7 +1897,7 @@
         <v>1.6711670051203247</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="F65" s="1"/>
     </row>

</xml_diff>